<commit_message>
planilla excel con datos de viga que verifica todo
</commit_message>
<xml_diff>
--- a/src/beam_diagnostic_system/resources/beamDataFile.xlsx
+++ b/src/beam_diagnostic_system/resources/beamDataFile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="216" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="432" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,20 +15,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>calidadAcero</t>
   </si>
   <si>
+    <t>Mpa</t>
+  </si>
+  <si>
     <t>calidadHormigon</t>
   </si>
   <si>
     <t>longitud</t>
   </si>
   <si>
+    <t>cm</t>
+  </si>
+  <si>
     <t>areaAcero</t>
   </si>
   <si>
+    <t>cm2</t>
+  </si>
+  <si>
     <t>altura</t>
   </si>
   <si>
@@ -45,6 +54,9 @@
   </si>
   <si>
     <t>corteUltimo</t>
+  </si>
+  <si>
+    <t>KN</t>
   </si>
   <si>
     <t>corteNominal</t>
@@ -66,7 +78,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,6 +99,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,9 +150,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -154,10 +177,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -171,111 +194,151 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="n">
-        <v>4</v>
+        <v>412</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>20</v>
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>7</v>
+        <v>747442</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>8</v>
+        <v>830500</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>9</v>
+        <v>174</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>10</v>
+        <v>232</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>11</v>
+        <v>0.4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>12</v>
+        <v>0.8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agrego reglas para elegir refuerzo
</commit_message>
<xml_diff>
--- a/src/beam_diagnostic_system/resources/beamDataFile.xlsx
+++ b/src/beam_diagnostic_system/resources/beamDataFile.xlsx
@@ -180,7 +180,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:C14"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -291,7 +291,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Puede dar como resultado, la misma viga o el refuerzo a usar o solucion inviable
</commit_message>
<xml_diff>
--- a/src/beam_diagnostic_system/resources/beamDataFile.xlsx
+++ b/src/beam_diagnostic_system/resources/beamDataFile.xlsx
@@ -180,7 +180,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -291,7 +291,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
agrego archivos de entrada que sirven como casos de uso
</commit_message>
<xml_diff>
--- a/src/beam_diagnostic_system/resources/beamDataFile.xlsx
+++ b/src/beam_diagnostic_system/resources/beamDataFile.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>calidadAcero</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>KN</t>
+  </si>
+  <si>
+    <t>CASO VIGA BIEN DIMENSIONADA</t>
   </si>
   <si>
     <t>corteNominal</t>
@@ -78,7 +81,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -103,6 +106,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF3333"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -150,13 +161,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -168,6 +183,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -177,10 +252,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -291,15 +366,18 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>232</v>
@@ -310,7 +388,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.4</v>
@@ -321,7 +399,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.8</v>
@@ -332,7 +410,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>5</v>

</xml_diff>